<commit_message>
Some LSS files updated
</commit_message>
<xml_diff>
--- a/T41_LSS/T41 Robotshop XBee V01.xlsx
+++ b/T41_LSS/T41 Robotshop XBee V01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Teensy3.1-Breakout-Boards\T41_LSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D304DA-D4B3-4995-9162-E1B66221FB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCED9E8B-9AE1-45A3-B31B-AFAC603B7730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16995" yWindow="7785" windowWidth="21180" windowHeight="12885" xr2:uid="{8F8CD82A-AA22-41B9-AB9B-E2F44D068376}"/>
   </bookViews>
@@ -790,7 +790,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>